<commit_message>
add models without overfitting
</commit_message>
<xml_diff>
--- a/0_data/7_models/comparison_model_stats.xlsx
+++ b/0_data/7_models/comparison_model_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,7 +531,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a1</t>
+          <t>a1_50</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -564,25 +564,25 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>717.6662</v>
+        <v>633.0726</v>
       </c>
       <c r="M2" t="n">
-        <v>11.96</v>
+        <v>10.55</v>
       </c>
       <c r="N2" t="n">
-        <v>1.373842477798462</v>
+        <v>1.341614484786987</v>
       </c>
       <c r="O2" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="P2" t="n">
-        <v>423.1065673828125</v>
+        <v>400.4725646972656</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.26</v>
+        <v>0.21</v>
       </c>
       <c r="R2" t="n">
-        <v>322.08</v>
+        <v>321.04</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
@@ -594,7 +594,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>a2</t>
+          <t>a2_50</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -627,25 +627,25 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>716.0189</v>
+        <v>660.1042</v>
       </c>
       <c r="M3" t="n">
-        <v>11.93</v>
+        <v>11</v>
       </c>
       <c r="N3" t="n">
-        <v>1.140858173370361</v>
+        <v>1.133472442626953</v>
       </c>
       <c r="O3" t="n">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="P3" t="n">
-        <v>472.513916015625</v>
+        <v>206.3318634033203</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.28</v>
+        <v>0.25</v>
       </c>
       <c r="R3" t="n">
-        <v>280.23</v>
+        <v>285.16</v>
       </c>
       <c r="S3" t="n">
         <v>1</v>
@@ -657,7 +657,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>a3</t>
+          <t>a3_50</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -690,25 +690,25 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>696.7114</v>
+        <v>636.4971</v>
       </c>
       <c r="M4" t="n">
-        <v>11.61</v>
+        <v>10.61</v>
       </c>
       <c r="N4" t="n">
-        <v>1.342280507087708</v>
+        <v>1.348449468612671</v>
       </c>
       <c r="O4" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="P4" t="n">
-        <v>252.6724548339844</v>
+        <v>167.7512664794922</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.14</v>
+        <v>0.25</v>
       </c>
       <c r="R4" t="n">
-        <v>320.89</v>
+        <v>319.93</v>
       </c>
       <c r="S4" t="n">
         <v>1</v>
@@ -720,7 +720,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>b_50</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -753,25 +753,25 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>636.9317</v>
+        <v>636.4864</v>
       </c>
       <c r="M5" t="n">
-        <v>10.62</v>
+        <v>10.61</v>
       </c>
       <c r="N5" t="n">
-        <v>1.32516884803772</v>
+        <v>1.349513411521912</v>
       </c>
       <c r="O5" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="P5" t="n">
-        <v>306.1823120117188</v>
+        <v>254.3524932861328</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.43</v>
+        <v>0.4</v>
       </c>
       <c r="R5" t="n">
-        <v>322.02</v>
+        <v>321.09</v>
       </c>
       <c r="S5" t="n">
         <v>1</v>
@@ -783,7 +783,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>c_50</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -816,25 +816,25 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>656.049</v>
+        <v>669.2868</v>
       </c>
       <c r="M6" t="n">
-        <v>10.93</v>
+        <v>11.15</v>
       </c>
       <c r="N6" t="n">
-        <v>1.362022161483765</v>
+        <v>1.340455532073975</v>
       </c>
       <c r="O6" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="P6" t="n">
-        <v>810.2303466796875</v>
+        <v>163.3970031738281</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.34</v>
+        <v>0.28</v>
       </c>
       <c r="R6" t="n">
-        <v>321.72</v>
+        <v>320.76</v>
       </c>
       <c r="S6" t="n">
         <v>1</v>
@@ -846,7 +846,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>d_50</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>598.8393</v>
+        <v>655.01</v>
       </c>
       <c r="M7" t="n">
-        <v>9.98</v>
+        <v>10.92</v>
       </c>
       <c r="N7" t="n">
         <v>1.167734980583191</v>
@@ -894,12 +894,390 @@
         <v>486.1801452636719</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.39</v>
+        <v>0.34</v>
       </c>
       <c r="R7" t="n">
-        <v>282.52</v>
+        <v>278.31</v>
       </c>
       <c r="S7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D8" t="n">
+        <v>256</v>
+      </c>
+      <c r="E8" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" t="n">
+        <v>6</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I8" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" t="n">
+        <v>4</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L8" t="n">
+        <v>265.258</v>
+      </c>
+      <c r="M8" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1.345364928245544</v>
+      </c>
+      <c r="O8" t="n">
+        <v>20</v>
+      </c>
+      <c r="P8" t="n">
+        <v>137.91455078125</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="R8" t="n">
+        <v>321.32</v>
+      </c>
+      <c r="S8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>a2</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D9" t="n">
+        <v>256</v>
+      </c>
+      <c r="E9" t="n">
+        <v>4</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>20</v>
+      </c>
+      <c r="J9" t="n">
+        <v>4</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L9" t="n">
+        <v>260.7209</v>
+      </c>
+      <c r="M9" t="n">
+        <v>4.35</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.202785968780518</v>
+      </c>
+      <c r="O9" t="n">
+        <v>20</v>
+      </c>
+      <c r="P9" t="n">
+        <v>120.4608306884766</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="R9" t="n">
+        <v>280.73</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>a3</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D10" t="n">
+        <v>256</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="n">
+        <v>6</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I10" t="n">
+        <v>20</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L10" t="n">
+        <v>262.6342</v>
+      </c>
+      <c r="M10" t="n">
+        <v>4.38</v>
+      </c>
+      <c r="N10" t="n">
+        <v>1.377196192741394</v>
+      </c>
+      <c r="O10" t="n">
+        <v>20</v>
+      </c>
+      <c r="P10" t="n">
+        <v>177.4877624511719</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="R10" t="n">
+        <v>321.58</v>
+      </c>
+      <c r="S10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D11" t="n">
+        <v>256</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I11" t="n">
+        <v>20</v>
+      </c>
+      <c r="J11" t="n">
+        <v>4</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L11" t="n">
+        <v>265.6575</v>
+      </c>
+      <c r="M11" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.343576550483704</v>
+      </c>
+      <c r="O11" t="n">
+        <v>20</v>
+      </c>
+      <c r="P11" t="n">
+        <v>188.3482666015625</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="R11" t="n">
+        <v>322.53</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D12" t="n">
+        <v>256</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>6</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I12" t="n">
+        <v>20</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L12" t="n">
+        <v>267.9921</v>
+      </c>
+      <c r="M12" t="n">
+        <v>4.47</v>
+      </c>
+      <c r="N12" t="n">
+        <v>1.347642779350281</v>
+      </c>
+      <c r="O12" t="n">
+        <v>20</v>
+      </c>
+      <c r="P12" t="n">
+        <v>138.1145477294922</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="R12" t="n">
+        <v>321.44</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D13" t="n">
+        <v>256</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I13" t="n">
+        <v>20</v>
+      </c>
+      <c r="J13" t="n">
+        <v>4</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L13" t="n">
+        <v>255.7635</v>
+      </c>
+      <c r="M13" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="N13" t="n">
+        <v>1.210534691810608</v>
+      </c>
+      <c r="O13" t="n">
+        <v>20</v>
+      </c>
+      <c r="P13" t="n">
+        <v>399.2044982910156</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="R13" t="n">
+        <v>285.27</v>
+      </c>
+      <c r="S13" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
run new mdoels and predictions
</commit_message>
<xml_diff>
--- a/0_data/7_models/comparison_model_stats.xlsx
+++ b/0_data/7_models/comparison_model_stats.xlsx
@@ -564,25 +564,25 @@
         </is>
       </c>
       <c r="L2" t="n">
-        <v>633.0726</v>
+        <v>646.7671</v>
       </c>
       <c r="M2" t="n">
-        <v>10.55</v>
+        <v>10.78</v>
       </c>
       <c r="N2" t="n">
-        <v>1.341614484786987</v>
+        <v>1.346299648284912</v>
       </c>
       <c r="O2" t="n">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="P2" t="n">
-        <v>400.4725646972656</v>
+        <v>679.5245361328125</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.21</v>
+        <v>0.42</v>
       </c>
       <c r="R2" t="n">
-        <v>321.04</v>
+        <v>322.9</v>
       </c>
       <c r="S2" t="n">
         <v>1</v>
@@ -627,25 +627,25 @@
         </is>
       </c>
       <c r="L3" t="n">
-        <v>660.1042</v>
+        <v>631.2694</v>
       </c>
       <c r="M3" t="n">
-        <v>11</v>
+        <v>10.52</v>
       </c>
       <c r="N3" t="n">
-        <v>1.133472442626953</v>
+        <v>1.177220463752747</v>
       </c>
       <c r="O3" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="P3" t="n">
-        <v>206.3318634033203</v>
+        <v>289.3336791992188</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.25</v>
+        <v>0.36</v>
       </c>
       <c r="R3" t="n">
-        <v>285.16</v>
+        <v>281.15</v>
       </c>
       <c r="S3" t="n">
         <v>1</v>
@@ -690,25 +690,25 @@
         </is>
       </c>
       <c r="L4" t="n">
-        <v>636.4971</v>
+        <v>662.6886</v>
       </c>
       <c r="M4" t="n">
-        <v>10.61</v>
+        <v>11.04</v>
       </c>
       <c r="N4" t="n">
-        <v>1.348449468612671</v>
+        <v>1.39044713973999</v>
       </c>
       <c r="O4" t="n">
         <v>36</v>
       </c>
       <c r="P4" t="n">
-        <v>167.7512664794922</v>
+        <v>275.9371032714844</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="R4" t="n">
-        <v>319.93</v>
+        <v>321.41</v>
       </c>
       <c r="S4" t="n">
         <v>1</v>
@@ -753,25 +753,25 @@
         </is>
       </c>
       <c r="L5" t="n">
-        <v>636.4864</v>
+        <v>652.5901</v>
       </c>
       <c r="M5" t="n">
-        <v>10.61</v>
+        <v>10.88</v>
       </c>
       <c r="N5" t="n">
-        <v>1.349513411521912</v>
+        <v>1.352879524230957</v>
       </c>
       <c r="O5" t="n">
         <v>36</v>
       </c>
       <c r="P5" t="n">
-        <v>254.3524932861328</v>
+        <v>442.3336181640625</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4</v>
+        <v>0.24</v>
       </c>
       <c r="R5" t="n">
-        <v>321.09</v>
+        <v>322.21</v>
       </c>
       <c r="S5" t="n">
         <v>1</v>
@@ -816,25 +816,25 @@
         </is>
       </c>
       <c r="L6" t="n">
-        <v>669.2868</v>
+        <v>643.5783</v>
       </c>
       <c r="M6" t="n">
-        <v>11.15</v>
+        <v>10.73</v>
       </c>
       <c r="N6" t="n">
-        <v>1.340455532073975</v>
+        <v>1.369530200958252</v>
       </c>
       <c r="O6" t="n">
         <v>36</v>
       </c>
       <c r="P6" t="n">
-        <v>163.3970031738281</v>
+        <v>364.7864074707031</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.28</v>
+        <v>0.32</v>
       </c>
       <c r="R6" t="n">
-        <v>320.76</v>
+        <v>321.04</v>
       </c>
       <c r="S6" t="n">
         <v>1</v>
@@ -879,10 +879,10 @@
         </is>
       </c>
       <c r="L7" t="n">
-        <v>655.01</v>
+        <v>634.2541</v>
       </c>
       <c r="M7" t="n">
-        <v>10.92</v>
+        <v>10.57</v>
       </c>
       <c r="N7" t="n">
         <v>1.167734980583191</v>
@@ -894,10 +894,10 @@
         <v>486.1801452636719</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.34</v>
+        <v>0.29</v>
       </c>
       <c r="R7" t="n">
-        <v>278.31</v>
+        <v>278.94</v>
       </c>
       <c r="S7" t="n">
         <v>1</v>
@@ -942,25 +942,25 @@
         </is>
       </c>
       <c r="L8" t="n">
-        <v>265.258</v>
+        <v>253.2759</v>
       </c>
       <c r="M8" t="n">
-        <v>4.42</v>
+        <v>4.22</v>
       </c>
       <c r="N8" t="n">
-        <v>1.345364928245544</v>
+        <v>1.378125429153442</v>
       </c>
       <c r="O8" t="n">
         <v>20</v>
       </c>
       <c r="P8" t="n">
-        <v>137.91455078125</v>
+        <v>94.86763763427734</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.45</v>
+        <v>0.55</v>
       </c>
       <c r="R8" t="n">
-        <v>321.32</v>
+        <v>322.85</v>
       </c>
       <c r="S8" t="n">
         <v>1</v>
@@ -1005,25 +1005,25 @@
         </is>
       </c>
       <c r="L9" t="n">
-        <v>260.7209</v>
+        <v>262.6371</v>
       </c>
       <c r="M9" t="n">
-        <v>4.35</v>
+        <v>4.38</v>
       </c>
       <c r="N9" t="n">
-        <v>1.202785968780518</v>
+        <v>1.272294044494629</v>
       </c>
       <c r="O9" t="n">
         <v>20</v>
       </c>
       <c r="P9" t="n">
-        <v>120.4608306884766</v>
+        <v>103.4351272583008</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.24</v>
+        <v>0.46</v>
       </c>
       <c r="R9" t="n">
-        <v>280.73</v>
+        <v>278.76</v>
       </c>
       <c r="S9" t="n">
         <v>1</v>
@@ -1068,25 +1068,25 @@
         </is>
       </c>
       <c r="L10" t="n">
-        <v>262.6342</v>
+        <v>263.4213</v>
       </c>
       <c r="M10" t="n">
-        <v>4.38</v>
+        <v>4.39</v>
       </c>
       <c r="N10" t="n">
-        <v>1.377196192741394</v>
+        <v>1.408199310302734</v>
       </c>
       <c r="O10" t="n">
         <v>20</v>
       </c>
       <c r="P10" t="n">
-        <v>177.4877624511719</v>
+        <v>202.8026733398438</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="R10" t="n">
-        <v>321.58</v>
+        <v>321.03</v>
       </c>
       <c r="S10" t="n">
         <v>1</v>
@@ -1131,25 +1131,25 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>265.6575</v>
+        <v>263.1353</v>
       </c>
       <c r="M11" t="n">
-        <v>4.43</v>
+        <v>4.39</v>
       </c>
       <c r="N11" t="n">
-        <v>1.343576550483704</v>
+        <v>1.351377487182617</v>
       </c>
       <c r="O11" t="n">
         <v>20</v>
       </c>
       <c r="P11" t="n">
-        <v>188.3482666015625</v>
+        <v>88.05629730224609</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.27</v>
+        <v>0.58</v>
       </c>
       <c r="R11" t="n">
-        <v>322.53</v>
+        <v>321.76</v>
       </c>
       <c r="S11" t="n">
         <v>1</v>
@@ -1194,25 +1194,25 @@
         </is>
       </c>
       <c r="L12" t="n">
-        <v>267.9921</v>
+        <v>253.012</v>
       </c>
       <c r="M12" t="n">
-        <v>4.47</v>
+        <v>4.22</v>
       </c>
       <c r="N12" t="n">
-        <v>1.347642779350281</v>
+        <v>1.394977211952209</v>
       </c>
       <c r="O12" t="n">
         <v>20</v>
       </c>
       <c r="P12" t="n">
-        <v>138.1145477294922</v>
+        <v>133.4529876708984</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.26</v>
+        <v>0.35</v>
       </c>
       <c r="R12" t="n">
-        <v>321.44</v>
+        <v>320.87</v>
       </c>
       <c r="S12" t="n">
         <v>1</v>
@@ -1257,10 +1257,10 @@
         </is>
       </c>
       <c r="L13" t="n">
-        <v>255.7635</v>
+        <v>260.3884</v>
       </c>
       <c r="M13" t="n">
-        <v>4.26</v>
+        <v>4.34</v>
       </c>
       <c r="N13" t="n">
         <v>1.210534691810608</v>
@@ -1272,10 +1272,10 @@
         <v>399.2044982910156</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="R13" t="n">
-        <v>285.27</v>
+        <v>275.16</v>
       </c>
       <c r="S13" t="n">
         <v>1</v>

</xml_diff>